<commit_message>
repository and script cleaning for public repository
</commit_message>
<xml_diff>
--- a/results/Supporting information/Table S1. Incubators detailed programs.xlsx
+++ b/results/Supporting information/Table S1. Incubators detailed programs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/movealong/results/Supplementary/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://unioviedo-my.sharepoint.com/personal/espinosaclara_uniovi_es/Documents/IMIB/Softwares/GitHub/Germination_phenology/results/Supporting information/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9C47C40-A5F7-44D1-823D-E1E0A1B10A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="8_{F9C47C40-A5F7-44D1-823D-E1E0A1B10A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB9B9946-545C-4554-AC2E-F0A20F144A19}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A69D5E9-DBB4-4953-9E9B-49E768234ACE}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1A69D5E9-DBB4-4953-9E9B-49E768234ACE}"/>
   </bookViews>
   <sheets>
     <sheet name="incubators programs" sheetId="1" r:id="rId1"/>
@@ -285,12 +285,6 @@
     <t xml:space="preserve">31 - 35 </t>
   </si>
   <si>
-    <t>Snowbed T</t>
-  </si>
-  <si>
-    <t>Fellfield T</t>
-  </si>
-  <si>
     <t>time (min)</t>
   </si>
   <si>
@@ -316,6 +310,12 @@
   </si>
   <si>
     <t>Week</t>
+  </si>
+  <si>
+    <t>Fellfield (TºC)</t>
+  </si>
+  <si>
+    <t>Snowbed (TºC)</t>
   </si>
 </sst>
 </file>
@@ -762,12 +762,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -797,9 +791,6 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="22" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -817,6 +808,15 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -839,9 +839,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -879,7 +879,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -985,7 +985,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1127,7 +1127,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1138,7 +1138,7 @@
   <dimension ref="A1:M176"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="E1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1151,8 +1151,8 @@
     <col min="8" max="8" width="11.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="10.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="5" customWidth="1"/>
     <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="14" bestFit="1" customWidth="1"/>
@@ -1167,52 +1167,52 @@
     <col min="25" max="25" width="6.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="43" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="43" t="s">
+    <row r="1" spans="1:12" s="40" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" s="46" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" s="46" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>80</v>
+      </c>
+      <c r="G1" s="44" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" s="44" t="s">
+        <v>78</v>
+      </c>
+      <c r="I1" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" s="43" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="L1" s="41" t="s">
         <v>86</v>
       </c>
-      <c r="C1" s="49" t="s">
-        <v>85</v>
-      </c>
-      <c r="D1" s="49" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" s="48" t="s">
-        <v>83</v>
-      </c>
-      <c r="F1" s="47" t="s">
-        <v>82</v>
-      </c>
-      <c r="G1" s="47" t="s">
-        <v>81</v>
-      </c>
-      <c r="H1" s="47" t="s">
-        <v>80</v>
-      </c>
-      <c r="I1" s="47" t="s">
-        <v>79</v>
-      </c>
-      <c r="J1" s="46" t="s">
-        <v>78</v>
-      </c>
-      <c r="K1" s="45" t="s">
-        <v>77</v>
-      </c>
-      <c r="L1" s="44" t="s">
-        <v>76</v>
-      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A2" s="38" t="s">
+      <c r="A2" s="36" t="s">
         <v>46</v>
       </c>
       <c r="B2">
         <v>2</v>
       </c>
-      <c r="C2" s="37">
+      <c r="C2" s="35">
         <v>-2</v>
       </c>
-      <c r="D2" s="37">
+      <c r="D2" s="35">
         <v>-1</v>
       </c>
       <c r="E2" s="20" t="s">
@@ -1241,16 +1241,16 @@
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="36" t="s">
         <v>46</v>
       </c>
       <c r="B3">
         <v>3</v>
       </c>
-      <c r="C3" s="37">
+      <c r="C3" s="35">
         <v>-1</v>
       </c>
-      <c r="D3" s="37">
+      <c r="D3" s="35">
         <v>-1</v>
       </c>
       <c r="E3" s="14" t="s">
@@ -1279,16 +1279,16 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="34" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="35">
+      <c r="B4" s="33">
         <v>4</v>
       </c>
-      <c r="C4" s="34">
+      <c r="C4" s="32">
         <v>-2</v>
       </c>
-      <c r="D4" s="34">
+      <c r="D4" s="32">
         <v>-1</v>
       </c>
       <c r="E4" s="8"/>
@@ -1315,16 +1315,16 @@
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="39" t="s">
         <v>72</v>
       </c>
-      <c r="B5" s="40">
+      <c r="B5" s="38">
         <v>5</v>
       </c>
-      <c r="C5" s="39">
+      <c r="C5" s="37">
         <v>-1</v>
       </c>
-      <c r="D5" s="39">
+      <c r="D5" s="37">
         <v>0</v>
       </c>
       <c r="E5" s="20">
@@ -1353,16 +1353,16 @@
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A6" s="38" t="s">
+      <c r="A6" s="36" t="s">
         <v>72</v>
       </c>
       <c r="B6">
         <v>6</v>
       </c>
-      <c r="C6" s="37">
+      <c r="C6" s="35">
         <v>-2</v>
       </c>
-      <c r="D6" s="37">
+      <c r="D6" s="35">
         <v>-1</v>
       </c>
       <c r="E6" s="14" t="s">
@@ -1391,16 +1391,16 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="38" t="s">
+      <c r="A7" s="36" t="s">
         <v>72</v>
       </c>
       <c r="B7">
         <v>7</v>
       </c>
-      <c r="C7" s="37">
+      <c r="C7" s="35">
         <v>-2</v>
       </c>
-      <c r="D7" s="37">
+      <c r="D7" s="35">
         <v>-1</v>
       </c>
       <c r="E7" s="8"/>
@@ -1427,16 +1427,16 @@
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="34" t="s">
         <v>72</v>
       </c>
-      <c r="B8" s="35">
+      <c r="B8" s="33">
         <v>8</v>
       </c>
-      <c r="C8" s="34">
+      <c r="C8" s="32">
         <v>-1</v>
       </c>
-      <c r="D8" s="34">
+      <c r="D8" s="32">
         <v>-1</v>
       </c>
       <c r="E8" s="20">
@@ -1465,16 +1465,16 @@
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A9" s="41" t="s">
+      <c r="A9" s="39" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="40">
+      <c r="B9" s="38">
         <v>9</v>
       </c>
-      <c r="C9" s="39">
+      <c r="C9" s="37">
         <v>-1</v>
       </c>
-      <c r="D9" s="39">
+      <c r="D9" s="37">
         <v>0</v>
       </c>
       <c r="E9" s="14" t="s">
@@ -1503,16 +1503,16 @@
       </c>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="38" t="s">
+      <c r="A10" s="36" t="s">
         <v>44</v>
       </c>
       <c r="B10">
         <v>10</v>
       </c>
-      <c r="C10" s="37">
+      <c r="C10" s="35">
         <v>-1</v>
       </c>
-      <c r="D10" s="37">
+      <c r="D10" s="35">
         <v>0</v>
       </c>
       <c r="E10" s="8"/>
@@ -1539,16 +1539,16 @@
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A11" s="38" t="s">
+      <c r="A11" s="36" t="s">
         <v>44</v>
       </c>
       <c r="B11">
         <v>11</v>
       </c>
-      <c r="C11" s="37">
-        <v>0</v>
-      </c>
-      <c r="D11" s="37">
+      <c r="C11" s="35">
+        <v>0</v>
+      </c>
+      <c r="D11" s="35">
         <v>1</v>
       </c>
       <c r="E11" s="20">
@@ -1577,16 +1577,16 @@
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A12" s="38" t="s">
+      <c r="A12" s="36" t="s">
         <v>44</v>
       </c>
       <c r="B12">
         <v>12</v>
       </c>
-      <c r="C12" s="37">
-        <v>0</v>
-      </c>
-      <c r="D12" s="37">
+      <c r="C12" s="35">
+        <v>0</v>
+      </c>
+      <c r="D12" s="35">
         <v>1</v>
       </c>
       <c r="E12" s="14" t="s">
@@ -1615,16 +1615,16 @@
       </c>
     </row>
     <row r="13" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="36" t="s">
+      <c r="A13" s="34" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="35">
+      <c r="B13" s="33">
         <v>13</v>
       </c>
-      <c r="C13" s="34">
-        <v>1</v>
-      </c>
-      <c r="D13" s="34">
+      <c r="C13" s="32">
+        <v>1</v>
+      </c>
+      <c r="D13" s="32">
         <v>2</v>
       </c>
       <c r="E13" s="8"/>
@@ -1651,16 +1651,16 @@
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="B14" s="40">
+      <c r="B14" s="38">
         <v>14</v>
       </c>
-      <c r="C14" s="39">
-        <v>1</v>
-      </c>
-      <c r="D14" s="39">
+      <c r="C14" s="37">
+        <v>1</v>
+      </c>
+      <c r="D14" s="37">
         <v>4</v>
       </c>
       <c r="E14" s="20">
@@ -1689,16 +1689,16 @@
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="38" t="s">
+      <c r="A15" s="36" t="s">
         <v>43</v>
       </c>
       <c r="B15">
         <v>15</v>
       </c>
-      <c r="C15" s="37">
-        <v>2</v>
-      </c>
-      <c r="D15" s="37">
+      <c r="C15" s="35">
+        <v>2</v>
+      </c>
+      <c r="D15" s="35">
         <v>5</v>
       </c>
       <c r="E15" s="14" t="s">
@@ -1727,16 +1727,16 @@
       </c>
     </row>
     <row r="16" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="38" t="s">
+      <c r="A16" s="36" t="s">
         <v>43</v>
       </c>
       <c r="B16">
         <v>16</v>
       </c>
-      <c r="C16" s="37">
-        <v>3</v>
-      </c>
-      <c r="D16" s="37">
+      <c r="C16" s="35">
+        <v>3</v>
+      </c>
+      <c r="D16" s="35">
         <v>6</v>
       </c>
       <c r="E16" s="8"/>
@@ -1763,16 +1763,16 @@
       </c>
     </row>
     <row r="17" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="36" t="s">
+      <c r="A17" s="34" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="35">
+      <c r="B17" s="33">
         <v>17</v>
       </c>
-      <c r="C17" s="34">
-        <v>3</v>
-      </c>
-      <c r="D17" s="34">
+      <c r="C17" s="32">
+        <v>3</v>
+      </c>
+      <c r="D17" s="32">
         <v>6</v>
       </c>
       <c r="E17" s="20">
@@ -1801,16 +1801,16 @@
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A18" s="41" t="s">
+      <c r="A18" s="39" t="s">
         <v>41</v>
       </c>
-      <c r="B18" s="40">
+      <c r="B18" s="38">
         <v>18</v>
       </c>
-      <c r="C18" s="39">
+      <c r="C18" s="37">
         <v>4</v>
       </c>
-      <c r="D18" s="39">
+      <c r="D18" s="37">
         <v>8</v>
       </c>
       <c r="E18" s="14" t="s">
@@ -1839,16 +1839,16 @@
       </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="38" t="s">
+      <c r="A19" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B19">
         <v>19</v>
       </c>
-      <c r="C19" s="37">
+      <c r="C19" s="35">
         <v>6</v>
       </c>
-      <c r="D19" s="37">
+      <c r="D19" s="35">
         <v>11</v>
       </c>
       <c r="E19" s="8"/>
@@ -1875,16 +1875,16 @@
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" s="38" t="s">
+      <c r="A20" s="36" t="s">
         <v>41</v>
       </c>
       <c r="B20">
         <v>20</v>
       </c>
-      <c r="C20" s="37">
+      <c r="C20" s="35">
         <v>7</v>
       </c>
-      <c r="D20" s="37">
+      <c r="D20" s="35">
         <v>12</v>
       </c>
       <c r="E20" s="20">
@@ -1913,16 +1913,16 @@
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" s="36" t="s">
+      <c r="A21" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="35">
+      <c r="B21" s="33">
         <v>21</v>
       </c>
-      <c r="C21" s="34">
+      <c r="C21" s="32">
         <v>7</v>
       </c>
-      <c r="D21" s="34">
+      <c r="D21" s="32">
         <v>13</v>
       </c>
       <c r="E21" s="14" t="s">
@@ -1951,16 +1951,16 @@
       </c>
     </row>
     <row r="22" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="41" t="s">
+      <c r="A22" s="39" t="s">
         <v>40</v>
       </c>
-      <c r="B22" s="40">
+      <c r="B22" s="38">
         <v>22</v>
       </c>
-      <c r="C22" s="39">
+      <c r="C22" s="37">
         <v>8</v>
       </c>
-      <c r="D22" s="39">
+      <c r="D22" s="37">
         <v>14</v>
       </c>
       <c r="E22" s="8"/>
@@ -1987,16 +1987,16 @@
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" s="38" t="s">
+      <c r="A23" s="36" t="s">
         <v>40</v>
       </c>
       <c r="B23">
         <v>23</v>
       </c>
-      <c r="C23" s="37">
+      <c r="C23" s="35">
         <v>10</v>
       </c>
-      <c r="D23" s="37">
+      <c r="D23" s="35">
         <v>15</v>
       </c>
       <c r="E23" s="20">
@@ -2025,16 +2025,16 @@
       </c>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="38" t="s">
+      <c r="A24" s="36" t="s">
         <v>40</v>
       </c>
       <c r="B24">
         <v>24</v>
       </c>
-      <c r="C24" s="37">
+      <c r="C24" s="35">
         <v>10</v>
       </c>
-      <c r="D24" s="37">
+      <c r="D24" s="35">
         <v>15</v>
       </c>
       <c r="E24" s="14" t="s">
@@ -2063,16 +2063,16 @@
       </c>
     </row>
     <row r="25" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="36" t="s">
+      <c r="A25" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B25" s="35">
+      <c r="B25" s="33">
         <v>25</v>
       </c>
-      <c r="C25" s="34">
+      <c r="C25" s="32">
         <v>11</v>
       </c>
-      <c r="D25" s="34">
+      <c r="D25" s="32">
         <v>18</v>
       </c>
       <c r="E25" s="8"/>
@@ -2099,16 +2099,16 @@
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A26" s="41" t="s">
+      <c r="A26" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="B26" s="40">
+      <c r="B26" s="38">
         <v>26</v>
       </c>
-      <c r="C26" s="39">
+      <c r="C26" s="37">
         <v>13</v>
       </c>
-      <c r="D26" s="39">
+      <c r="D26" s="37">
         <v>19</v>
       </c>
       <c r="E26" s="20">
@@ -2137,16 +2137,16 @@
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A27" s="38" t="s">
+      <c r="A27" s="36" t="s">
         <v>38</v>
       </c>
       <c r="B27">
         <v>27</v>
       </c>
-      <c r="C27" s="37">
+      <c r="C27" s="35">
         <v>14</v>
       </c>
-      <c r="D27" s="37">
+      <c r="D27" s="35">
         <v>20</v>
       </c>
       <c r="E27" s="14" t="s">
@@ -2175,16 +2175,16 @@
       </c>
     </row>
     <row r="28" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="38" t="s">
+      <c r="A28" s="36" t="s">
         <v>38</v>
       </c>
       <c r="B28">
         <v>28</v>
       </c>
-      <c r="C28" s="37">
+      <c r="C28" s="35">
         <v>14</v>
       </c>
-      <c r="D28" s="37">
+      <c r="D28" s="35">
         <v>20</v>
       </c>
       <c r="E28" s="8"/>
@@ -2211,16 +2211,16 @@
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A29" s="38" t="s">
+      <c r="A29" s="36" t="s">
         <v>38</v>
       </c>
       <c r="B29">
         <v>29</v>
       </c>
-      <c r="C29" s="37">
+      <c r="C29" s="35">
         <v>15</v>
       </c>
-      <c r="D29" s="37">
+      <c r="D29" s="35">
         <v>21</v>
       </c>
       <c r="E29" s="20">
@@ -2249,16 +2249,16 @@
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="34" t="s">
         <v>38</v>
       </c>
-      <c r="B30" s="35">
+      <c r="B30" s="33">
         <v>30</v>
       </c>
-      <c r="C30" s="34">
+      <c r="C30" s="32">
         <v>15</v>
       </c>
-      <c r="D30" s="34">
+      <c r="D30" s="32">
         <v>21</v>
       </c>
       <c r="E30" s="14" t="s">
@@ -2287,16 +2287,16 @@
       </c>
     </row>
     <row r="31" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="41" t="s">
+      <c r="A31" s="39" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="40">
+      <c r="B31" s="38">
         <v>31</v>
       </c>
-      <c r="C31" s="39">
+      <c r="C31" s="37">
         <v>15</v>
       </c>
-      <c r="D31" s="39">
+      <c r="D31" s="37">
         <v>21</v>
       </c>
       <c r="E31" s="8"/>
@@ -2323,16 +2323,16 @@
       </c>
     </row>
     <row r="32" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="38" t="s">
+      <c r="A32" s="36" t="s">
         <v>36</v>
       </c>
       <c r="B32">
         <v>32</v>
       </c>
-      <c r="C32" s="37">
+      <c r="C32" s="35">
         <v>14</v>
       </c>
-      <c r="D32" s="37">
+      <c r="D32" s="35">
         <v>21</v>
       </c>
       <c r="E32" s="20">
@@ -2361,16 +2361,16 @@
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="38" t="s">
+      <c r="A33" s="36" t="s">
         <v>36</v>
       </c>
       <c r="B33">
         <v>33</v>
       </c>
-      <c r="C33" s="37">
+      <c r="C33" s="35">
         <v>15</v>
       </c>
-      <c r="D33" s="37">
+      <c r="D33" s="35">
         <v>21</v>
       </c>
       <c r="E33" s="14" t="s">
@@ -2399,16 +2399,16 @@
       </c>
     </row>
     <row r="34" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="36" t="s">
+      <c r="A34" s="34" t="s">
         <v>36</v>
       </c>
-      <c r="B34" s="35">
+      <c r="B34" s="33">
         <v>34</v>
       </c>
-      <c r="C34" s="34">
+      <c r="C34" s="32">
         <v>16</v>
       </c>
-      <c r="D34" s="34">
+      <c r="D34" s="32">
         <v>21</v>
       </c>
       <c r="E34" s="8"/>
@@ -2435,16 +2435,16 @@
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="41" t="s">
+      <c r="A35" s="39" t="s">
         <v>35</v>
       </c>
-      <c r="B35" s="40">
+      <c r="B35" s="38">
         <v>35</v>
       </c>
-      <c r="C35" s="39">
+      <c r="C35" s="37">
         <v>14</v>
       </c>
-      <c r="D35" s="39">
+      <c r="D35" s="37">
         <v>20</v>
       </c>
       <c r="E35" s="20">
@@ -2473,16 +2473,16 @@
       </c>
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="38" t="s">
+      <c r="A36" s="36" t="s">
         <v>35</v>
       </c>
       <c r="B36">
         <v>36</v>
       </c>
-      <c r="C36" s="37">
+      <c r="C36" s="35">
         <v>13</v>
       </c>
-      <c r="D36" s="37">
+      <c r="D36" s="35">
         <v>19</v>
       </c>
       <c r="E36" s="14" t="s">
@@ -2511,16 +2511,16 @@
       </c>
     </row>
     <row r="37" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="38" t="s">
+      <c r="A37" s="36" t="s">
         <v>35</v>
       </c>
       <c r="B37">
         <v>37</v>
       </c>
-      <c r="C37" s="37">
+      <c r="C37" s="35">
         <v>12</v>
       </c>
-      <c r="D37" s="37">
+      <c r="D37" s="35">
         <v>16</v>
       </c>
       <c r="E37" s="8"/>
@@ -2547,16 +2547,16 @@
       </c>
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A38" s="38" t="s">
+      <c r="A38" s="36" t="s">
         <v>35</v>
       </c>
       <c r="B38">
         <v>38</v>
       </c>
-      <c r="C38" s="37">
+      <c r="C38" s="35">
         <v>10</v>
       </c>
-      <c r="D38" s="37">
+      <c r="D38" s="35">
         <v>15</v>
       </c>
       <c r="E38" s="20">
@@ -2585,16 +2585,16 @@
       </c>
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A39" s="36" t="s">
+      <c r="A39" s="34" t="s">
         <v>35</v>
       </c>
-      <c r="B39" s="35">
+      <c r="B39" s="33">
         <v>39</v>
       </c>
-      <c r="C39" s="34">
+      <c r="C39" s="32">
         <v>9</v>
       </c>
-      <c r="D39" s="34">
+      <c r="D39" s="32">
         <v>14</v>
       </c>
       <c r="E39" s="14" t="s">
@@ -2623,52 +2623,52 @@
       </c>
     </row>
     <row r="40" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="41" t="s">
+      <c r="A40" s="39" t="s">
         <v>34</v>
       </c>
-      <c r="B40" s="40">
+      <c r="B40" s="38">
         <v>40</v>
       </c>
-      <c r="C40" s="39">
+      <c r="C40" s="37">
         <v>9</v>
       </c>
-      <c r="D40" s="39">
+      <c r="D40" s="37">
         <v>13</v>
       </c>
-      <c r="E40" s="32"/>
-      <c r="F40" s="31">
-        <v>3</v>
-      </c>
-      <c r="G40" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="H40" s="30">
+      <c r="E40" s="30"/>
+      <c r="F40" s="29">
+        <v>3</v>
+      </c>
+      <c r="G40" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H40" s="28">
         <v>0.62569444444444444</v>
       </c>
-      <c r="I40" s="30">
+      <c r="I40" s="28">
         <v>0.75</v>
       </c>
-      <c r="J40" s="29">
+      <c r="J40" s="27">
         <v>180</v>
       </c>
-      <c r="K40" s="28">
+      <c r="K40" s="26">
         <v>2.5</v>
       </c>
-      <c r="L40" s="27">
+      <c r="L40" s="25">
         <v>0.5</v>
       </c>
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A41" s="38" t="s">
+      <c r="A41" s="36" t="s">
         <v>34</v>
       </c>
       <c r="B41">
         <v>41</v>
       </c>
-      <c r="C41" s="37">
+      <c r="C41" s="35">
         <v>8</v>
       </c>
-      <c r="D41" s="37">
+      <c r="D41" s="35">
         <v>11</v>
       </c>
       <c r="E41" s="20" t="s">
@@ -2695,21 +2695,21 @@
       <c r="L41" s="24">
         <v>0</v>
       </c>
-      <c r="M41" s="42" t="s">
+      <c r="M41" s="47" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A42" s="38" t="s">
+      <c r="A42" s="36" t="s">
         <v>34</v>
       </c>
       <c r="B42">
         <v>42</v>
       </c>
-      <c r="C42" s="37">
+      <c r="C42" s="35">
         <v>6</v>
       </c>
-      <c r="D42" s="37">
+      <c r="D42" s="35">
         <v>9</v>
       </c>
       <c r="E42" s="14" t="s">
@@ -2736,19 +2736,19 @@
       <c r="L42" s="9">
         <v>0</v>
       </c>
-      <c r="M42" s="26"/>
+      <c r="M42" s="48"/>
     </row>
     <row r="43" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="36" t="s">
+      <c r="A43" s="34" t="s">
         <v>34</v>
       </c>
-      <c r="B43" s="35">
+      <c r="B43" s="33">
         <v>43</v>
       </c>
-      <c r="C43" s="34">
+      <c r="C43" s="32">
         <v>5</v>
       </c>
-      <c r="D43" s="34">
+      <c r="D43" s="32">
         <v>8</v>
       </c>
       <c r="E43" s="8"/>
@@ -2773,19 +2773,19 @@
       <c r="L43" s="23">
         <v>0</v>
       </c>
-      <c r="M43" s="26"/>
+      <c r="M43" s="48"/>
     </row>
     <row r="44" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A44" s="41" t="s">
+      <c r="A44" s="39" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="40">
+      <c r="B44" s="38">
         <v>44</v>
       </c>
-      <c r="C44" s="39">
+      <c r="C44" s="37">
         <v>4</v>
       </c>
-      <c r="D44" s="39">
+      <c r="D44" s="37">
         <v>6</v>
       </c>
       <c r="E44" s="20" t="s">
@@ -2812,19 +2812,19 @@
       <c r="L44" s="24">
         <v>0</v>
       </c>
-      <c r="M44" s="26"/>
+      <c r="M44" s="48"/>
     </row>
     <row r="45" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A45" s="38" t="s">
+      <c r="A45" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B45">
         <v>45</v>
       </c>
-      <c r="C45" s="37">
-        <v>3</v>
-      </c>
-      <c r="D45" s="37">
+      <c r="C45" s="35">
+        <v>3</v>
+      </c>
+      <c r="D45" s="35">
         <v>4</v>
       </c>
       <c r="E45" s="14" t="s">
@@ -2851,19 +2851,19 @@
       <c r="L45" s="9">
         <v>0</v>
       </c>
-      <c r="M45" s="26"/>
+      <c r="M45" s="48"/>
     </row>
     <row r="46" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="38" t="s">
+      <c r="A46" s="36" t="s">
         <v>32</v>
       </c>
       <c r="B46">
         <v>46</v>
       </c>
-      <c r="C46" s="37">
-        <v>2</v>
-      </c>
-      <c r="D46" s="37">
+      <c r="C46" s="35">
+        <v>2</v>
+      </c>
+      <c r="D46" s="35">
         <v>4</v>
       </c>
       <c r="E46" s="8"/>
@@ -2888,19 +2888,19 @@
       <c r="L46" s="23">
         <v>0</v>
       </c>
-      <c r="M46" s="26"/>
+      <c r="M46" s="48"/>
     </row>
     <row r="47" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A47" s="36" t="s">
+      <c r="A47" s="34" t="s">
         <v>32</v>
       </c>
-      <c r="B47" s="35">
+      <c r="B47" s="33">
         <v>47</v>
       </c>
-      <c r="C47" s="34">
-        <v>2</v>
-      </c>
-      <c r="D47" s="34">
+      <c r="C47" s="32">
+        <v>2</v>
+      </c>
+      <c r="D47" s="32">
         <v>3</v>
       </c>
       <c r="E47" s="20">
@@ -2927,19 +2927,19 @@
       <c r="L47" s="24">
         <v>0</v>
       </c>
-      <c r="M47" s="26"/>
+      <c r="M47" s="48"/>
     </row>
     <row r="48" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="41" t="s">
+      <c r="A48" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B48" s="40">
+      <c r="B48" s="38">
         <v>48</v>
       </c>
-      <c r="C48" s="39">
-        <v>0</v>
-      </c>
-      <c r="D48" s="39">
+      <c r="C48" s="37">
+        <v>0</v>
+      </c>
+      <c r="D48" s="37">
         <v>1</v>
       </c>
       <c r="E48" s="8" t="s">
@@ -2966,22 +2966,22 @@
       <c r="L48" s="23">
         <v>0</v>
       </c>
-      <c r="M48" s="26"/>
+      <c r="M48" s="48"/>
     </row>
     <row r="49" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="38" t="s">
+      <c r="A49" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B49">
         <v>49</v>
       </c>
-      <c r="C49" s="37">
-        <v>0</v>
-      </c>
-      <c r="D49" s="37">
-        <v>1</v>
-      </c>
-      <c r="E49" s="33" t="s">
+      <c r="C49" s="35">
+        <v>0</v>
+      </c>
+      <c r="D49" s="35">
+        <v>1</v>
+      </c>
+      <c r="E49" s="31" t="s">
         <v>54</v>
       </c>
       <c r="F49" s="19">
@@ -3005,19 +3005,19 @@
       <c r="L49" s="24">
         <v>0</v>
       </c>
-      <c r="M49" s="26"/>
+      <c r="M49" s="48"/>
     </row>
     <row r="50" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A50" s="38" t="s">
+      <c r="A50" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B50">
         <v>50</v>
       </c>
-      <c r="C50" s="37">
+      <c r="C50" s="35">
         <v>-1</v>
       </c>
-      <c r="D50" s="37">
+      <c r="D50" s="35">
         <v>0</v>
       </c>
       <c r="E50" s="14" t="s">
@@ -3044,56 +3044,56 @@
       <c r="L50" s="9">
         <v>0</v>
       </c>
-      <c r="M50" s="26"/>
+      <c r="M50" s="48"/>
     </row>
     <row r="51" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="38" t="s">
+      <c r="A51" s="36" t="s">
         <v>30</v>
       </c>
       <c r="B51">
         <v>51</v>
       </c>
-      <c r="C51" s="37">
+      <c r="C51" s="35">
         <v>-1</v>
       </c>
-      <c r="D51" s="37">
-        <v>0</v>
-      </c>
-      <c r="E51" s="32"/>
-      <c r="F51" s="31">
-        <v>3</v>
-      </c>
-      <c r="G51" s="31" t="s">
+      <c r="D51" s="35">
+        <v>0</v>
+      </c>
+      <c r="E51" s="30"/>
+      <c r="F51" s="29">
+        <v>3</v>
+      </c>
+      <c r="G51" s="29" t="s">
         <v>45</v>
       </c>
-      <c r="H51" s="30">
+      <c r="H51" s="28">
         <v>0.62569444444444444</v>
       </c>
-      <c r="I51" s="30">
+      <c r="I51" s="28">
         <v>0.70833333333333337</v>
       </c>
-      <c r="J51" s="29">
+      <c r="J51" s="27">
         <v>120</v>
       </c>
-      <c r="K51" s="28">
+      <c r="K51" s="26">
         <v>-1.5</v>
       </c>
-      <c r="L51" s="27">
-        <v>0</v>
-      </c>
-      <c r="M51" s="26"/>
+      <c r="L51" s="25">
+        <v>0</v>
+      </c>
+      <c r="M51" s="48"/>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A52" s="36" t="s">
+      <c r="A52" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B52" s="35">
+      <c r="B52" s="33">
         <v>52</v>
       </c>
-      <c r="C52" s="34">
+      <c r="C52" s="32">
         <v>-1</v>
       </c>
-      <c r="D52" s="34">
+      <c r="D52" s="32">
         <v>-1</v>
       </c>
       <c r="E52" s="20">
@@ -3120,7 +3120,7 @@
       <c r="L52" s="24">
         <v>0</v>
       </c>
-      <c r="M52" s="26"/>
+      <c r="M52" s="48"/>
     </row>
     <row r="53" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E53" s="8" t="s">
@@ -3147,7 +3147,7 @@
       <c r="L53" s="23">
         <v>0</v>
       </c>
-      <c r="M53" s="26"/>
+      <c r="M53" s="48"/>
     </row>
     <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
@@ -3180,7 +3180,7 @@
       <c r="L54" s="24">
         <v>0</v>
       </c>
-      <c r="M54" s="26"/>
+      <c r="M54" s="48"/>
     </row>
     <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
@@ -3213,7 +3213,7 @@
       <c r="L55" s="9">
         <v>0</v>
       </c>
-      <c r="M55" s="26"/>
+      <c r="M55" s="48"/>
     </row>
     <row r="56" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
@@ -3247,7 +3247,7 @@
       <c r="L56" s="23">
         <v>0</v>
       </c>
-      <c r="M56" s="26"/>
+      <c r="M56" s="48"/>
     </row>
     <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
@@ -3283,7 +3283,7 @@
       <c r="L57" s="24">
         <v>0</v>
       </c>
-      <c r="M57" s="26"/>
+      <c r="M57" s="48"/>
     </row>
     <row r="58" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
@@ -3319,7 +3319,7 @@
       <c r="L58" s="9">
         <v>0</v>
       </c>
-      <c r="M58" s="26"/>
+      <c r="M58" s="48"/>
     </row>
     <row r="59" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
@@ -3353,7 +3353,7 @@
       <c r="L59" s="23">
         <v>0</v>
       </c>
-      <c r="M59" s="26"/>
+      <c r="M59" s="48"/>
     </row>
     <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
@@ -3365,7 +3365,7 @@
       <c r="C60">
         <v>15.5</v>
       </c>
-      <c r="E60" s="33" t="s">
+      <c r="E60" s="31" t="s">
         <v>39</v>
       </c>
       <c r="F60" s="19">
@@ -3389,7 +3389,7 @@
       <c r="L60" s="24">
         <v>0</v>
       </c>
-      <c r="M60" s="26"/>
+      <c r="M60" s="48"/>
     </row>
     <row r="61" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
@@ -3425,7 +3425,7 @@
       <c r="L61" s="9">
         <v>0</v>
       </c>
-      <c r="M61" s="26"/>
+      <c r="M61" s="48"/>
     </row>
     <row r="62" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
@@ -3459,7 +3459,7 @@
       <c r="L62" s="23">
         <v>0</v>
       </c>
-      <c r="M62" s="26"/>
+      <c r="M62" s="48"/>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
@@ -3495,7 +3495,7 @@
       <c r="L63" s="24">
         <v>0</v>
       </c>
-      <c r="M63" s="26"/>
+      <c r="M63" s="48"/>
     </row>
     <row r="64" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
@@ -3531,7 +3531,7 @@
       <c r="L64" s="23">
         <v>0</v>
       </c>
-      <c r="M64" s="26"/>
+      <c r="M64" s="48"/>
     </row>
     <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
@@ -3543,7 +3543,7 @@
       <c r="C65">
         <v>10</v>
       </c>
-      <c r="E65" s="33" t="s">
+      <c r="E65" s="31" t="s">
         <v>31</v>
       </c>
       <c r="F65" s="19">
@@ -3567,7 +3567,7 @@
       <c r="L65" s="24">
         <v>0</v>
       </c>
-      <c r="M65" s="26"/>
+      <c r="M65" s="48"/>
     </row>
     <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
@@ -3603,7 +3603,7 @@
       <c r="L66" s="9">
         <v>0</v>
       </c>
-      <c r="M66" s="26"/>
+      <c r="M66" s="48"/>
     </row>
     <row r="67" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E67" s="8"/>
@@ -3628,10 +3628,10 @@
       <c r="L67" s="23">
         <v>0</v>
       </c>
-      <c r="M67" s="26"/>
+      <c r="M67" s="48"/>
     </row>
     <row r="68" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E68" s="33" t="s">
+      <c r="E68" s="31" t="s">
         <v>28</v>
       </c>
       <c r="F68" s="19">
@@ -3655,7 +3655,7 @@
       <c r="L68" s="24">
         <v>0</v>
       </c>
-      <c r="M68" s="26"/>
+      <c r="M68" s="48"/>
     </row>
     <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E69" s="14" t="s">
@@ -3682,7 +3682,7 @@
       <c r="L69" s="9">
         <v>0</v>
       </c>
-      <c r="M69" s="26"/>
+      <c r="M69" s="48"/>
     </row>
     <row r="70" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E70" s="8"/>
@@ -3707,7 +3707,7 @@
       <c r="L70" s="23">
         <v>0</v>
       </c>
-      <c r="M70" s="26"/>
+      <c r="M70" s="48"/>
     </row>
     <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E71" s="20">
@@ -3734,7 +3734,7 @@
       <c r="L71" s="24">
         <v>0</v>
       </c>
-      <c r="M71" s="26"/>
+      <c r="M71" s="48"/>
     </row>
     <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E72" s="14" t="s">
@@ -3761,7 +3761,7 @@
       <c r="L72" s="9">
         <v>0</v>
       </c>
-      <c r="M72" s="26"/>
+      <c r="M72" s="48"/>
     </row>
     <row r="73" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E73" s="8"/>
@@ -3786,7 +3786,7 @@
       <c r="L73" s="23">
         <v>0</v>
       </c>
-      <c r="M73" s="26"/>
+      <c r="M73" s="48"/>
     </row>
     <row r="74" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E74" s="20">
@@ -3813,7 +3813,7 @@
       <c r="L74" s="24">
         <v>0</v>
       </c>
-      <c r="M74" s="26"/>
+      <c r="M74" s="48"/>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E75" s="14" t="s">
@@ -3840,7 +3840,7 @@
       <c r="L75" s="9">
         <v>0</v>
       </c>
-      <c r="M75" s="26"/>
+      <c r="M75" s="48"/>
     </row>
     <row r="76" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E76" s="8"/>
@@ -3865,7 +3865,7 @@
       <c r="L76" s="23">
         <v>0</v>
       </c>
-      <c r="M76" s="26"/>
+      <c r="M76" s="48"/>
     </row>
     <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E77" s="20">
@@ -3892,7 +3892,7 @@
       <c r="L77" s="24">
         <v>0</v>
       </c>
-      <c r="M77" s="26"/>
+      <c r="M77" s="48"/>
     </row>
     <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E78" s="14" t="s">
@@ -3919,7 +3919,7 @@
       <c r="L78" s="9">
         <v>0</v>
       </c>
-      <c r="M78" s="26"/>
+      <c r="M78" s="48"/>
     </row>
     <row r="79" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E79" s="8"/>
@@ -3944,7 +3944,7 @@
       <c r="L79" s="23">
         <v>0</v>
       </c>
-      <c r="M79" s="26"/>
+      <c r="M79" s="48"/>
     </row>
     <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E80" s="20" t="s">
@@ -3971,7 +3971,7 @@
       <c r="L80" s="24">
         <v>0</v>
       </c>
-      <c r="M80" s="26"/>
+      <c r="M80" s="48"/>
     </row>
     <row r="81" spans="5:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E81" s="14" t="s">
@@ -3998,7 +3998,7 @@
       <c r="L81" s="9">
         <v>0</v>
       </c>
-      <c r="M81" s="26"/>
+      <c r="M81" s="48"/>
     </row>
     <row r="82" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E82" s="8"/>
@@ -4023,7 +4023,7 @@
       <c r="L82" s="23">
         <v>0</v>
       </c>
-      <c r="M82" s="26"/>
+      <c r="M82" s="48"/>
     </row>
     <row r="83" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E83" s="20">
@@ -4050,7 +4050,7 @@
       <c r="L83" s="24">
         <v>0</v>
       </c>
-      <c r="M83" s="26"/>
+      <c r="M83" s="48"/>
     </row>
     <row r="84" spans="5:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E84" s="14" t="s">
@@ -4077,32 +4077,32 @@
       <c r="L84" s="9">
         <v>0</v>
       </c>
-      <c r="M84" s="26"/>
+      <c r="M84" s="48"/>
     </row>
     <row r="85" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E85" s="32"/>
-      <c r="F85" s="31">
-        <v>3</v>
-      </c>
-      <c r="G85" s="31" t="s">
-        <v>0</v>
-      </c>
-      <c r="H85" s="30">
+      <c r="E85" s="30"/>
+      <c r="F85" s="29">
+        <v>3</v>
+      </c>
+      <c r="G85" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H85" s="28">
         <v>0.62569444444444444</v>
       </c>
-      <c r="I85" s="30">
+      <c r="I85" s="28">
         <v>0.85416666666666663</v>
       </c>
-      <c r="J85" s="29">
+      <c r="J85" s="27">
         <v>330</v>
       </c>
-      <c r="K85" s="28">
+      <c r="K85" s="26">
         <v>6</v>
       </c>
-      <c r="L85" s="27">
-        <v>0</v>
-      </c>
-      <c r="M85" s="26"/>
+      <c r="L85" s="25">
+        <v>0</v>
+      </c>
+      <c r="M85" s="48"/>
     </row>
     <row r="86" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E86" s="20">
@@ -4129,7 +4129,7 @@
       <c r="L86" s="24">
         <v>0</v>
       </c>
-      <c r="M86" s="26"/>
+      <c r="M86" s="48"/>
     </row>
     <row r="87" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E87" s="14" t="s">
@@ -4156,7 +4156,7 @@
       <c r="L87" s="9">
         <v>0</v>
       </c>
-      <c r="M87" s="26"/>
+      <c r="M87" s="48"/>
     </row>
     <row r="88" spans="5:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="E88" s="8"/>
@@ -4181,7 +4181,7 @@
       <c r="L88" s="23">
         <v>0</v>
       </c>
-      <c r="M88" s="25"/>
+      <c r="M88" s="49"/>
     </row>
     <row r="89" spans="5:13" x14ac:dyDescent="0.25">
       <c r="E89" s="20">

</xml_diff>